<commit_message>
small edits to dataset analysis assignment
</commit_message>
<xml_diff>
--- a/assignments/dataset-biography-template.xlsx
+++ b/assignments/dataset-biography-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lxt308/Dropbox/Teaching/2021-spring/eng395-f20/syllabus-assignments/assignments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9594884F-66C3-D24F-94C1-BA36EB784BA2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502DBA3B-30C0-F144-A5BA-4A5D0FEFBCF9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="680" windowWidth="26320" windowHeight="12700" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>Dataset Name</t>
   </si>
@@ -124,6 +124,12 @@
   </si>
   <si>
     <t>Link(s) to documentation of data and/or project</t>
+  </si>
+  <si>
+    <t>Who is the audience for this data?</t>
+  </si>
+  <si>
+    <t>researchers, policy makers</t>
   </si>
 </sst>
 </file>
@@ -485,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -499,10 +505,10 @@
     <col min="4" max="6" width="10.83203125" style="3"/>
     <col min="7" max="7" width="11.83203125" style="3" customWidth="1"/>
     <col min="8" max="8" width="15.83203125" style="3" customWidth="1"/>
-    <col min="9" max="13" width="10.83203125" style="3"/>
+    <col min="9" max="14" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -537,13 +543,16 @@
         <v>6</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="96" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="102" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -574,8 +583,11 @@
       <c r="K2" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="L2" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" ht="268" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="301" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
@@ -602,6 +614,9 @@
       </c>
       <c r="K3" s="3" t="s">
         <v>16</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
response papers 3 and 4 and dataset bio template
</commit_message>
<xml_diff>
--- a/assignments/dataset-biography-template.xlsx
+++ b/assignments/dataset-biography-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lxt308/Dropbox/Teaching/2021-spring/eng395-f20/syllabus-assignments/assignments/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lxt308/Dropbox/github/websites/teaching/eng395s21/assignments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502DBA3B-30C0-F144-A5BA-4A5D0FEFBCF9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A83306B4-68EE-4D42-B91B-462E2C2CFBA2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="680" windowWidth="26320" windowHeight="12700" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="680" windowWidth="29240" windowHeight="14680" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general info" sheetId="1" r:id="rId1"/>
@@ -126,10 +126,10 @@
     <t>Link(s) to documentation of data and/or project</t>
   </si>
   <si>
-    <t>Who is the audience for this data?</t>
-  </si>
-  <si>
     <t>researchers, policy makers</t>
+  </si>
+  <si>
+    <t>Who is the audience for this data</t>
   </si>
 </sst>
 </file>
@@ -493,8 +493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -543,7 +543,7 @@
         <v>6</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>7</v>
@@ -584,7 +584,7 @@
         <v>10</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="301" x14ac:dyDescent="0.2">
@@ -616,7 +616,7 @@
         <v>16</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>